<commit_message>
Add DIDO-POI.md, fix Dido equality.
</commit_message>
<xml_diff>
--- a/dido-poi/src/test/resources/excel/SimpleTableWithHeadings.xlsx
+++ b/dido-poi/src/test/resources/excel/SimpleTableWithHeadings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rob\projects\dido\dido-poi\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{72738323-DA11-43FE-B00A-E9E068D85070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811FCF5A-5E07-4597-9C77-B8CC65C040E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25695" yWindow="9495" windowWidth="17085" windowHeight="12600" xr2:uid="{A1AA1AFF-1410-4777-BEC8-8260879ED5F9}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" xr2:uid="{A1AA1AFF-1410-4777-BEC8-8260879ED5F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Fruit</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>Pear</t>
+  </si>
+  <si>
+    <t>BestBefore</t>
   </si>
 </sst>
 </file>
@@ -89,8 +92,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,15 +429,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CE146E5-6857-42FC-AF40-8CE4AFC540C3}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="13.109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -443,8 +450,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -454,8 +464,11 @@
       <c r="C2">
         <v>23.5</v>
       </c>
+      <c r="D2" s="1">
+        <v>45615</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -465,8 +478,11 @@
       <c r="C3">
         <v>47.2</v>
       </c>
+      <c r="D3" s="1">
+        <v>45631</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -475,6 +491,9 @@
       </c>
       <c r="C4">
         <v>34.200000000000003</v>
+      </c>
+      <c r="D4" s="1">
+        <v>45665</v>
       </c>
     </row>
   </sheetData>

</xml_diff>